<commit_message>
1) Proactive error prevention for numerical instability, 2) Proper handling of missing annotation data
</commit_message>
<xml_diff>
--- a/R/alcohol_intake_frequency/ADH1C.xlsx
+++ b/R/alcohol_intake_frequency/ADH1C.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Gene name</t>
   </si>
@@ -95,16 +95,58 @@
     <t>plof</t>
   </si>
   <si>
+    <t>0.212043039500717</t>
+  </si>
+  <si>
+    <t>0.000118663512438457</t>
+  </si>
+  <si>
+    <t>0.21198221670806</t>
+  </si>
+  <si>
+    <t>3.1420857957681e-16</t>
+  </si>
+  <si>
+    <t>3.14216389575831e-16</t>
+  </si>
+  <si>
+    <t>0.0312960738135757</t>
+  </si>
+  <si>
+    <t>0.000557259935895171</t>
+  </si>
+  <si>
+    <t>0.00109511334597734</t>
+  </si>
+  <si>
+    <t>0.00109504743955036</t>
+  </si>
+  <si>
+    <t>4.44089209850063e-16</t>
+  </si>
+  <si>
+    <t>1.11022302462516e-15</t>
+  </si>
+  <si>
+    <t>1.33226762955019e-15</t>
+  </si>
+  <si>
     <t>ptv</t>
   </si>
   <si>
     <t>synonymous</t>
   </si>
   <si>
+    <t>6.04219080496842e-169</t>
+  </si>
+  <si>
     <t>ptv_ds</t>
   </si>
   <si>
     <t>missense</t>
+  </si>
+  <si>
+    <t>3.37133641153819e-216</t>
   </si>
 </sst>
 </file>
@@ -720,20 +762,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1271,8 +1307,8 @@
   <sheetPr/>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:S1"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T$1:AE$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.55752212389381" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -1280,23 +1316,19 @@
     <col min="1" max="1" width="10.5929203539823" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.53097345132743" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.7256637168142" style="1" customWidth="1"/>
-    <col min="4" max="5" width="5.53097345132743" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6637168141593" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7964601769912" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6637168141593" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.929203539823" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7964601769912" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.929203539823" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7964601769912" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.0619469026549" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.929203539823" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.0619469026549" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.929203539823" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.0619469026549" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.929203539823" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5929203539823" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.53097345132743" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.55752212389381" style="1"/>
+    <col min="4" max="4" width="5.53097345132743" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.53097345132743" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.9911504424779" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.858407079646" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5221238938053" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.3893805309735" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.787610619469" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.858407079646" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.9911504424779" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.858407079646" style="1" customWidth="1"/>
+    <col min="14" max="15" width="21.787610619469" style="1" customWidth="1"/>
+    <col min="16" max="19" width="22.858407079646" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.55752212389381" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1315,46 +1347,46 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1369,52 +1401,52 @@
         <v>20</v>
       </c>
       <c r="D2" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1">
-        <v>35</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.000118665463447772</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.21198221670806</v>
-      </c>
-      <c r="J2" s="4">
-        <v>3.1420857957681e-16</v>
-      </c>
-      <c r="K2" s="4">
-        <v>3.14216389575831e-16</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0.0014756878090405</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0.00099182706861245</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.00118635271703893</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0.00118628122232578</v>
-      </c>
-      <c r="P2" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="R2" s="4">
-        <v>1.11022302462516e-15</v>
-      </c>
-      <c r="S2" s="4">
-        <v>1.33226762955019e-15</v>
+        <v>9459</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1433,47 +1465,47 @@
       <c r="E3" s="1">
         <v>35</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.000118663512438457</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.21198221670806</v>
-      </c>
-      <c r="J3" s="4">
-        <v>3.1420857957681e-16</v>
-      </c>
-      <c r="K3" s="4">
-        <v>3.14216389575831e-16</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0.0312960738135757</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0.000557259935895171</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.00109511334597734</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0.00109504743955036</v>
-      </c>
-      <c r="P3" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="R3" s="4">
-        <v>1.11022302462516e-15</v>
-      </c>
-      <c r="S3" s="4">
-        <v>1.33226762955019e-15</v>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1484,55 +1516,55 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.000118665463447772</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.21198221670806</v>
-      </c>
-      <c r="J4" s="4">
-        <v>3.1420857957681e-16</v>
-      </c>
-      <c r="K4" s="4">
-        <v>3.14216389575831e-16</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.0014756878090405</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.00099182706861245</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.00118635271703893</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.00118628122232578</v>
-      </c>
-      <c r="P4" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1.11022302462516e-15</v>
-      </c>
-      <c r="S4" s="4">
-        <v>1.33226762955019e-15</v>
+        <v>9578</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1543,55 +1575,55 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1">
-        <v>1189</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3.07249597036361e-149</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.89480744701012e-207</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1.89768581903258e-213</v>
-      </c>
-      <c r="I5" s="4">
-        <v>2.20325810050513e-213</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1.00661019833561e-74</v>
-      </c>
-      <c r="K5" s="4">
-        <v>1.00390635360752e-74</v>
-      </c>
-      <c r="L5" s="4">
-        <v>5.28097854088464e-184</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1.20899241899511e-241</v>
-      </c>
-      <c r="N5" s="4">
-        <v>2.69398877312254e-231</v>
-      </c>
-      <c r="O5" s="4">
-        <v>3.46820607094002e-231</v>
-      </c>
-      <c r="P5" s="4">
-        <v>1.07061993549538e-74</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>1.06771338446888e-74</v>
-      </c>
-      <c r="R5" s="4">
-        <v>6.11726109522441e-213</v>
-      </c>
-      <c r="S5" s="4">
-        <v>7.25395451339224e-241</v>
+        <v>12856</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1602,55 +1634,55 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1">
-        <v>35</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.000118665463447772</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.212043039500717</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.21198221670806</v>
-      </c>
-      <c r="J6" s="4">
-        <v>3.1420857957681e-16</v>
-      </c>
-      <c r="K6" s="4">
-        <v>3.14216389575831e-16</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0.0014756878090405</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.00099182706861245</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.00118635271703893</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.00118628122232578</v>
-      </c>
-      <c r="P6" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>4.44089209850063e-16</v>
-      </c>
-      <c r="R6" s="4">
-        <v>1.11022302462516e-15</v>
-      </c>
-      <c r="S6" s="4">
-        <v>1.33226762955019e-15</v>
+        <v>9578</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1661,52 +1693,52 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E7" s="1">
-        <v>1747</v>
-      </c>
-      <c r="F7" s="4">
-        <v>6.08057757491721e-215</v>
-      </c>
-      <c r="G7" s="4">
-        <v>2.31902948460133e-233</v>
-      </c>
-      <c r="H7" s="4">
-        <v>2.50677290210639e-167</v>
-      </c>
-      <c r="I7" s="4">
-        <v>5.28675376891142e-167</v>
-      </c>
-      <c r="J7" s="4">
-        <v>4.16905052618687e-90</v>
-      </c>
-      <c r="K7" s="4">
-        <v>4.16864725249558e-90</v>
-      </c>
-      <c r="L7" s="4">
-        <v>2.43021164447739e-244</v>
+        <v>4364</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
       </c>
-      <c r="N7" s="4">
-        <v>2.25971474893443e-210</v>
-      </c>
-      <c r="O7" s="4">
-        <v>3.95626395624107e-210</v>
-      </c>
-      <c r="P7" s="4">
-        <v>4.25725958531375e-90</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>4.25682368358542e-90</v>
-      </c>
-      <c r="R7" s="4">
-        <v>1.3914176907608e-232</v>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
       </c>
       <c r="S7" s="1">
         <v>0</v>

</xml_diff>